<commit_message>
Vuelvo a subir todo, todo hecho. Fala revisar, mezclar lances para optimizar umbral y que sea más visual, y cambiar el gráfico de umbral de datos mixtos
</commit_message>
<xml_diff>
--- a/resultados/mix_predicciones_percent.xlsx
+++ b/resultados/mix_predicciones_percent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t xml:space="preserve">Predicted by model</t>
   </si>
@@ -104,18 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%SKJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%BET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%YFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%FRI </t>
   </si>
   <si>
     <t xml:space="preserve">%SKJ_N</t>
@@ -287,7 +275,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,7 +332,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,7 +420,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -635,35 +627,27 @@
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="I11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="M11" s="10"/>
       <c r="U11" s="10"/>
@@ -672,18 +656,10 @@
       <c r="A12" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B12" s="12" t="n">
-        <v>0.11543536179404</v>
-      </c>
-      <c r="C12" s="12" t="n">
-        <v>0.561252877106325</v>
-      </c>
-      <c r="D12" s="12" t="n">
-        <v>0.323311761099636</v>
-      </c>
-      <c r="E12" s="12" t="n">
-        <v>0</v>
-      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="13" t="n">
         <v>0.19672131147541</v>
       </c>
@@ -697,10 +673,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M12" s="10"/>
       <c r="U12" s="10"/>
@@ -709,18 +685,10 @@
       <c r="A13" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B13" s="12" t="n">
-        <v>0.516838760913098</v>
-      </c>
-      <c r="C13" s="12" t="n">
-        <v>0.2055328234248</v>
-      </c>
-      <c r="D13" s="12" t="n">
-        <v>0.272253821099946</v>
-      </c>
-      <c r="E13" s="12" t="n">
-        <v>0.00537459456215601</v>
-      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="13" t="n">
         <v>0.652830188679245</v>
       </c>
@@ -734,13 +702,13 @@
         <v>0.0113207547169811</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="M13" s="10"/>
       <c r="U13" s="10"/>
@@ -777,13 +745,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="14" t="n">
+        <v>0.19672131147541</v>
+      </c>
+      <c r="D17" s="14" t="n">
+        <v>0.311475409836066</v>
+      </c>
+      <c r="E17" s="14" t="n">
+        <v>0.491803278688525</v>
+      </c>
+      <c r="F17" s="14" t="n">
+        <v>0.652830188679245</v>
+      </c>
+      <c r="G17" s="14" t="n">
+        <v>0.169811320754717</v>
+      </c>
+      <c r="H17" s="14" t="n">
+        <v>0.166037735849057</v>
+      </c>
+      <c r="I17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>